<commit_message>
updata db en wireframe
</commit_message>
<xml_diff>
--- a/sql/nadenkendatabank.xlsx
+++ b/sql/nadenkendatabank.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="18195" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>tblstudent</t>
   </si>
@@ -51,9 +56,6 @@
     <t>elk vak in tblvakken heeft een begin- en einduur</t>
   </si>
   <si>
-    <t>tussentabel</t>
-  </si>
-  <si>
     <t>tblvakken</t>
   </si>
   <si>
@@ -64,9 +66,6 @@
   </si>
   <si>
     <t>tbldagen</t>
-  </si>
-  <si>
-    <t>tbl klassen</t>
   </si>
   <si>
     <t>klas id</t>
@@ -175,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +187,20 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -247,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -264,9 +277,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -572,31 +587,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
@@ -608,13 +623,13 @@
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -622,7 +637,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5">
         <v>0.35416666666666669</v>
@@ -634,21 +649,21 @@
         <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5">
         <v>0.39583333333333331</v>
@@ -660,21 +675,18 @@
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="5">
         <v>0.44791666666666669</v>
@@ -684,15 +696,15 @@
       </c>
       <c r="I4" s="4"/>
       <c r="K4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="G5" s="5">
         <v>0.48958333333333331</v>
@@ -702,15 +714,18 @@
       </c>
       <c r="I5" s="4"/>
       <c r="K5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="G6" s="5">
         <v>0.57291666666666663</v>
@@ -720,15 +735,18 @@
       </c>
       <c r="I6" s="4"/>
       <c r="K6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5">
         <v>0.61458333333333337</v>
@@ -738,9 +756,12 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
+      <c r="C8" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G8" s="5">
         <v>0.66666666666666663</v>
@@ -750,7 +771,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="G9" s="5">
         <v>0.70833333333333337</v>
       </c>
@@ -759,49 +780,36 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
+    <row r="11" spans="1:13">
       <c r="G11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19" s="8">
         <v>1</v>
@@ -816,35 +824,35 @@
         <v>4</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="I20" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3"/>
       <c r="E21" s="8">
@@ -860,12 +868,12 @@
         <v>5</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22" s="8">
         <v>2</v>
@@ -880,10 +888,10 @@
         <v>8</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -900,10 +908,10 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -920,10 +928,10 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="E25" s="8">
         <v>5</v>
       </c>
@@ -939,7 +947,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -949,9 +962,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -961,8 +979,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>